<commit_message>
More clear explanition for our second method and more details about results of experiment
</commit_message>
<xml_diff>
--- a/statistic/result.xlsx
+++ b/statistic/result.xlsx
@@ -12806,8 +12806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L37" sqref="K14:L37"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37:J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -12867,7 +12867,7 @@
         <v>88.838782412599997</v>
       </c>
       <c r="H2" s="3">
-        <v>92.446448703499996</v>
+        <v>91.431792559200005</v>
       </c>
       <c r="I2" s="3">
         <v>89.639639639600006</v>
@@ -12899,7 +12899,7 @@
         <v>89.064261555800002</v>
       </c>
       <c r="H3" s="3">
-        <v>92.671927846700001</v>
+        <v>91.995490417100001</v>
       </c>
       <c r="I3" s="3">
         <v>90.990990991000004</v>
@@ -12931,7 +12931,7 @@
         <v>91.544532130800008</v>
       </c>
       <c r="H4" s="3">
-        <v>93.235625704599997</v>
+        <v>92.446448703499996</v>
       </c>
       <c r="I4" s="3">
         <v>90.540540540500004</v>
@@ -12963,7 +12963,7 @@
         <v>90.304396843300012</v>
       </c>
       <c r="H5" s="3">
-        <v>91.770011273999998</v>
+        <v>91.882750845499999</v>
       </c>
       <c r="I5" s="3">
         <v>89.414414414399999</v>
@@ -12995,7 +12995,7 @@
         <v>90.529875986500002</v>
       </c>
       <c r="H6" s="3">
-        <v>93.686583991000006</v>
+        <v>92.446448703499996</v>
       </c>
       <c r="I6" s="3">
         <v>88.963963964000001</v>
@@ -13027,7 +13027,7 @@
         <v>89.853438556900002</v>
       </c>
       <c r="H7" s="3">
-        <v>91.544532130799993</v>
+        <v>91.882750845499999</v>
       </c>
       <c r="I7" s="3">
         <v>90.090090090100006</v>
@@ -13059,7 +13059,7 @@
         <v>89.853438556900002</v>
       </c>
       <c r="H8" s="3">
-        <v>91.093573844399998</v>
+        <v>91.882750845499999</v>
       </c>
       <c r="I8" s="3">
         <v>90.315315315299998</v>
@@ -13091,7 +13091,7 @@
         <v>90.078917700100007</v>
       </c>
       <c r="H9" s="3">
-        <v>92.559188275099999</v>
+        <v>92.333709131899994</v>
       </c>
       <c r="I9" s="3">
         <v>91.216216216199996</v>
@@ -13123,7 +13123,7 @@
         <v>90.98083427280001</v>
       </c>
       <c r="H10" s="3">
-        <v>92.108229988700003</v>
+        <v>91.544532130799993</v>
       </c>
       <c r="I10" s="3">
         <v>93.693693693699998</v>
@@ -13155,7 +13155,7 @@
         <v>89.96617812849999</v>
       </c>
       <c r="H11" s="3">
-        <v>93.686583991000006</v>
+        <v>91.544532130799993</v>
       </c>
       <c r="I11" s="3">
         <v>89.414414414399999</v>
@@ -13187,7 +13187,7 @@
         <v>90.304396843300012</v>
       </c>
       <c r="H12" s="3">
-        <v>91.319052987600003</v>
+        <v>93.122886132999994</v>
       </c>
       <c r="I12" s="3">
         <v>90.990990991000004</v>
@@ -13219,7 +13219,7 @@
         <v>89.853438556900002</v>
       </c>
       <c r="H13" s="3">
-        <v>92.897406989900006</v>
+        <v>92.220969560300006</v>
       </c>
       <c r="I13" s="3">
         <v>89.639639639600006</v>
@@ -13251,7 +13251,7 @@
         <v>89.96617812849999</v>
       </c>
       <c r="H14" s="3">
-        <v>90.868094701199993</v>
+        <v>91.431792559200005</v>
       </c>
       <c r="I14" s="3">
         <v>89.864864864899999</v>
@@ -13283,7 +13283,7 @@
         <v>89.853438556900002</v>
       </c>
       <c r="H15" s="3">
-        <v>91.206313416</v>
+        <v>91.882750845499999</v>
       </c>
       <c r="I15" s="3">
         <v>91.666666666699996</v>
@@ -13315,7 +13315,7 @@
         <v>90.642615558100005</v>
       </c>
       <c r="H16" s="3">
-        <v>92.108229988700003</v>
+        <v>90.755355129700007</v>
       </c>
       <c r="I16" s="3">
         <v>93.693693693699998</v>
@@ -13347,7 +13347,7 @@
         <v>91.206313416</v>
       </c>
       <c r="H17" s="3">
-        <v>93.348365276199999</v>
+        <v>90.755355129700007</v>
       </c>
       <c r="I17" s="3">
         <v>90.765765765799998</v>
@@ -13379,7 +13379,7 @@
         <v>91.093573844399998</v>
       </c>
       <c r="H18" s="3">
-        <v>91.995490417100001</v>
+        <v>91.544532130799993</v>
       </c>
       <c r="I18" s="3">
         <v>91.216216216199996</v>
@@ -13411,7 +13411,7 @@
         <v>88.049605411499996</v>
       </c>
       <c r="H19" s="3">
-        <v>89.064261555800002</v>
+        <v>91.882750845499999</v>
       </c>
       <c r="I19" s="3">
         <v>90.540540540500004</v>
@@ -13443,7 +13443,7 @@
         <v>89.627959413799999</v>
       </c>
       <c r="H20" s="3">
-        <v>91.544532130799993</v>
+        <v>92.897406989900006</v>
       </c>
       <c r="I20" s="3">
         <v>92.117117117099994</v>
@@ -13475,7 +13475,7 @@
         <v>89.064261555800002</v>
       </c>
       <c r="H21" s="3">
-        <v>92.784667418300003</v>
+        <v>92.220969560300006</v>
       </c>
       <c r="I21" s="3">
         <v>88.738738738699993</v>
@@ -13507,7 +13507,7 @@
         <v>89.402480270600009</v>
       </c>
       <c r="H22" s="3">
-        <v>92.671927846700001</v>
+        <v>91.431792559200005</v>
       </c>
       <c r="I22" s="3">
         <v>89.639639639600006</v>
@@ -13539,7 +13539,7 @@
         <v>89.289740698999992</v>
       </c>
       <c r="H23" s="3">
-        <v>93.010146561400006</v>
+        <v>91.657271702399996</v>
       </c>
       <c r="I23" s="3">
         <v>90.315315315299998</v>
@@ -13571,7 +13571,7 @@
         <v>89.289740698999992</v>
       </c>
       <c r="H24" s="3">
-        <v>92.108229988700003</v>
+        <v>92.784667418300003</v>
       </c>
       <c r="I24" s="3">
         <v>88.738738738699993</v>
@@ -13603,7 +13603,7 @@
         <v>89.064261555800002</v>
       </c>
       <c r="H25" s="3">
-        <v>93.010146561400006</v>
+        <v>90.868094701199993</v>
       </c>
       <c r="I25" s="3">
         <v>91.666666666699996</v>
@@ -13635,7 +13635,7 @@
         <v>89.7406989853</v>
       </c>
       <c r="H26" s="3">
-        <v>92.446448703499996</v>
+        <v>91.995490417100001</v>
       </c>
       <c r="I26" s="3">
         <v>89.189189189199993</v>
@@ -13667,7 +13667,7 @@
         <v>91.093573844399998</v>
       </c>
       <c r="H27" s="3">
-        <v>92.784667418300003</v>
+        <v>91.882750845499999</v>
       </c>
       <c r="I27" s="3">
         <v>89.414414414399999</v>
@@ -13699,7 +13699,7 @@
         <v>89.7406989853</v>
       </c>
       <c r="H28" s="3">
-        <v>91.431792559200005</v>
+        <v>90.642615558100005</v>
       </c>
       <c r="I28" s="3">
         <v>89.864864864899999</v>
@@ -13731,7 +13731,7 @@
         <v>91.093573844399998</v>
       </c>
       <c r="H29" s="3">
-        <v>92.784667418300003</v>
+        <v>91.995490417100001</v>
       </c>
       <c r="I29" s="3">
         <v>90.540540540500004</v>
@@ -13763,7 +13763,7 @@
         <v>89.627959413799999</v>
       </c>
       <c r="H30" s="3">
-        <v>92.897406989900006</v>
+        <v>91.995490417100001</v>
       </c>
       <c r="I30" s="3">
         <v>88.963963964000001</v>
@@ -13795,7 +13795,7 @@
         <v>90.191657271699995</v>
       </c>
       <c r="H31" s="3">
-        <v>93.122886132999994</v>
+        <v>92.559188275099999</v>
       </c>
       <c r="I31" s="3">
         <v>90.990990991000004</v>
@@ -13834,7 +13834,7 @@
       </c>
       <c r="H33" s="3">
         <f t="shared" si="0"/>
-        <v>92.273581360393351</v>
+        <v>91.863960916943341</v>
       </c>
       <c r="I33" s="3">
         <f t="shared" ref="I33" si="1">AVERAGE(I2:I31)</f>
@@ -13875,7 +13875,7 @@
       </c>
       <c r="H34" s="3">
         <f t="shared" si="2"/>
-        <v>0.97914746333862723</v>
+        <v>0.61755920950648258</v>
       </c>
       <c r="I34" s="3">
         <f t="shared" ref="I34" si="3">STDEV(I2:I31)</f>
@@ -13892,1179 +13892,1179 @@
       </c>
       <c r="B35" s="3">
         <f>(AVERAGE(B37:B66)/STDEV(B37:B66))*SQRT(50)</f>
-        <v>2.2593405596586762</v>
+        <v>1.0577317769137531</v>
       </c>
       <c r="C35" s="3">
         <f>(AVERAGE(C37:C66)/STDEV(C37:C66))*SQRT(50)</f>
-        <v>3.1201545973854219</v>
+        <v>3.4077710054823713</v>
       </c>
       <c r="D35" s="3">
         <f t="shared" ref="D35:J35" si="4">(AVERAGE(D37:D66)/STDEV(D37:D66))*SQRT(50)</f>
-        <v>35.445981519806445</v>
+        <v>34.192428872385101</v>
       </c>
       <c r="E35" s="3">
         <f t="shared" si="4"/>
-        <v>8.9571327287969105</v>
+        <v>7.0728558916991835</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" si="4"/>
-        <v>26.056766198207505</v>
+        <v>25.637036744923122</v>
       </c>
       <c r="G35" s="3">
         <f t="shared" si="4"/>
-        <v>15.925705958927008</v>
-      </c>
-      <c r="H35" s="3" t="e">
+        <v>11.934600314310837</v>
+      </c>
+      <c r="H35" s="3">
+        <f t="shared" si="4"/>
+        <v>0.34063500243371553</v>
+      </c>
+      <c r="I35" s="3">
+        <f t="shared" si="4"/>
+        <v>7.1477409755261654</v>
+      </c>
+      <c r="J35" s="3" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I35" s="3">
-        <f t="shared" si="4"/>
-        <v>7.4658937079731533</v>
-      </c>
-      <c r="J35" s="3">
-        <f t="shared" si="4"/>
-        <v>2.0517040099870703</v>
-      </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B37" s="3">
-        <f>H2-B2</f>
-        <v>-0.1127395715845978</v>
+        <f>J2-B2</f>
+        <v>-0.45095828635859903</v>
       </c>
       <c r="C37" s="3">
-        <f>H2-C2</f>
-        <v>0.33821871477400123</v>
+        <f>J2-C2</f>
+        <v>0</v>
       </c>
       <c r="D37" s="3">
-        <f>H2-D2</f>
-        <v>5.2987598647000027</v>
+        <f>J2-D2</f>
+        <v>4.9605411499260015</v>
       </c>
       <c r="E37" s="3">
-        <f>H2-E2</f>
-        <v>0.9019165727221008</v>
+        <f>J2-E2</f>
+        <v>0.56369785794809957</v>
       </c>
       <c r="F37" s="3">
-        <f>H2-F2</f>
-        <v>5.2987598647000027</v>
+        <f>J2-F2</f>
+        <v>4.9605411499260015</v>
       </c>
       <c r="G37" s="3">
-        <f>H2-G2</f>
-        <v>3.6076662908999992</v>
+        <f>J2-G2</f>
+        <v>3.269447576125998</v>
       </c>
       <c r="H37" s="3">
-        <f>H2-H2</f>
-        <v>0</v>
+        <f>J2-H2</f>
+        <v>0.67643742952598984</v>
       </c>
       <c r="I37" s="3">
-        <f>H2-I2</f>
-        <v>2.8068090638999905</v>
+        <f>J2-I2</f>
+        <v>2.4685903491259893</v>
       </c>
       <c r="J37" s="3">
-        <f>H2-J2</f>
-        <v>0.33821871477400123</v>
+        <f>J2-J2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B38" s="3">
-        <f t="shared" ref="B38:B66" si="5">H3-B3</f>
-        <v>2.5806912162806839E-11</v>
+        <f t="shared" ref="B38:B66" si="5">J3-B3</f>
+        <v>-1.3528748590754986</v>
       </c>
       <c r="C38" s="3">
-        <f t="shared" ref="C38:C66" si="6">H3-C3</f>
-        <v>0.45095828638430646</v>
+        <f t="shared" ref="C38:C66" si="6">J3-C3</f>
+        <v>-0.9019165727169991</v>
       </c>
       <c r="D38" s="3">
-        <f t="shared" ref="D38:D66" si="7">H3-D3</f>
-        <v>6.7643742954000032</v>
+        <f t="shared" ref="D38:D66" si="7">J3-D3</f>
+        <v>5.4114994362986977</v>
       </c>
       <c r="E38" s="3">
-        <f t="shared" ref="E38:E66" si="8">H3-E3</f>
-        <v>1.1273957159221055</v>
+        <f t="shared" ref="E38:E66" si="8">J3-E3</f>
+        <v>-0.22547914317920004</v>
       </c>
       <c r="F38" s="3">
-        <f t="shared" ref="F38:F66" si="9">H3-F3</f>
-        <v>4.5095828636000022</v>
+        <f t="shared" ref="F38:F66" si="9">J3-F3</f>
+        <v>3.1567080044986966</v>
       </c>
       <c r="G38" s="3">
-        <f t="shared" ref="G38:G66" si="10">H3-G3</f>
-        <v>3.6076662908999992</v>
+        <f t="shared" ref="G38:G66" si="10">J3-G3</f>
+        <v>2.2547914317986937</v>
       </c>
       <c r="H38" s="3">
-        <f t="shared" ref="H38:H66" si="11">H3-H3</f>
-        <v>0</v>
+        <f t="shared" ref="H38:H66" si="11">J3-H3</f>
+        <v>-0.67643742950130559</v>
       </c>
       <c r="I38" s="3">
-        <f t="shared" ref="I38:I66" si="12">H3-I3</f>
-        <v>1.6809368556999971</v>
+        <f t="shared" ref="I38:I66" si="12">J3-I3</f>
+        <v>0.32806199659869151</v>
       </c>
       <c r="J38" s="3">
-        <f t="shared" ref="J38:J66" si="13">H3-J3</f>
-        <v>1.3528748591013056</v>
+        <f t="shared" ref="J38:J66" si="13">J3-J3</f>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B39" s="3">
         <f t="shared" si="5"/>
-        <v>1.6910935738221013</v>
+        <v>0.78917700112739908</v>
       </c>
       <c r="C39" s="3">
         <f t="shared" si="6"/>
-        <v>1.2401352874636018</v>
+        <v>0.33821871476889953</v>
       </c>
       <c r="D39" s="3">
         <f t="shared" si="7"/>
-        <v>7.2153325816999967</v>
+        <v>6.3134160090052944</v>
       </c>
       <c r="E39" s="3">
         <f t="shared" si="8"/>
-        <v>2.7057497181287005</v>
+        <v>1.8038331454339982</v>
       </c>
       <c r="F39" s="3">
         <f t="shared" si="9"/>
-        <v>6.2006764373999914</v>
+        <v>5.2987598647052891</v>
       </c>
       <c r="G39" s="3">
         <f t="shared" si="10"/>
-        <v>1.6910935737999893</v>
+        <v>0.78917700110528699</v>
       </c>
       <c r="H39" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-0.11273957159470172</v>
       </c>
       <c r="I39" s="3">
         <f t="shared" si="12"/>
-        <v>2.6950851640999929</v>
+        <v>1.7931685914052906</v>
       </c>
       <c r="J39" s="3">
         <f t="shared" si="13"/>
-        <v>0.90191657269470227</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B40" s="3">
         <f t="shared" si="5"/>
-        <v>1.2401352875287017</v>
+        <v>0</v>
       </c>
       <c r="C40" s="3">
         <f t="shared" si="6"/>
-        <v>1.1273957159391017</v>
+        <v>-0.11273957158960002</v>
       </c>
       <c r="D40" s="3">
         <f t="shared" si="7"/>
-        <v>4.9605411499999974</v>
+        <v>3.7204058624712957</v>
       </c>
       <c r="E40" s="3">
         <f t="shared" si="8"/>
-        <v>2.8184892897834999</v>
+        <v>1.5783540022547982</v>
       </c>
       <c r="F40" s="3">
         <f t="shared" si="9"/>
-        <v>4.6223224352000045</v>
+        <v>3.3821871476713028</v>
       </c>
       <c r="G40" s="3">
         <f t="shared" si="10"/>
-        <v>1.4656144306999863</v>
+        <v>0.22547914317128459</v>
       </c>
       <c r="H40" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-1.3528748590287023</v>
       </c>
       <c r="I40" s="3">
         <f t="shared" si="12"/>
-        <v>2.3555968595999985</v>
+        <v>1.1154615720712968</v>
       </c>
       <c r="J40" s="3">
         <f t="shared" si="13"/>
-        <v>1.2401352875287017</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B41" s="3">
         <f t="shared" si="5"/>
-        <v>1.3528748590947117</v>
+        <v>1.1273957158962986</v>
       </c>
       <c r="C41" s="3">
         <f t="shared" si="6"/>
-        <v>1.6910935738636113</v>
+        <v>1.4656144306651981</v>
       </c>
       <c r="D41" s="3">
         <f t="shared" si="7"/>
-        <v>9.9210822999000072</v>
+        <v>9.6956031567015941</v>
       </c>
       <c r="E41" s="3">
         <f t="shared" si="8"/>
-        <v>4.396843292014708</v>
+        <v>4.1713641488162949</v>
       </c>
       <c r="F41" s="3">
         <f t="shared" si="9"/>
-        <v>4.8478015784000092</v>
+        <v>4.6223224352015961</v>
       </c>
       <c r="G41" s="3">
         <f t="shared" si="10"/>
-        <v>3.156708004500004</v>
+        <v>2.9312288613015909</v>
       </c>
       <c r="H41" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.0146561443015969</v>
       </c>
       <c r="I41" s="3">
         <f t="shared" si="12"/>
-        <v>4.7226200270000049</v>
+        <v>4.4971408838015918</v>
       </c>
       <c r="J41" s="3">
         <f t="shared" si="13"/>
-        <v>0.22547914319841311</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B42" s="3">
         <f t="shared" si="5"/>
-        <v>-2.5930101465394131</v>
+        <v>-2.1420518602030114</v>
       </c>
       <c r="C42" s="3">
         <f t="shared" si="6"/>
-        <v>-1.3528748590534008</v>
+        <v>-0.9019165727169991</v>
       </c>
       <c r="D42" s="3">
         <f t="shared" si="7"/>
-        <v>6.8771138669999914</v>
+        <v>7.3280721533363931</v>
       </c>
       <c r="E42" s="3">
         <f t="shared" si="8"/>
-        <v>1.465614430687296</v>
+        <v>1.9165727170236977</v>
       </c>
       <c r="F42" s="3">
         <f t="shared" si="9"/>
-        <v>2.7057497181999963</v>
+        <v>3.156708004536398</v>
       </c>
       <c r="G42" s="3">
         <f t="shared" si="10"/>
-        <v>1.691093573899991</v>
+        <v>2.1420518602363927</v>
       </c>
       <c r="H42" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.11273957163639636</v>
       </c>
       <c r="I42" s="3">
         <f t="shared" si="12"/>
-        <v>1.4544420406999876</v>
+        <v>1.9054003270363893</v>
       </c>
       <c r="J42" s="3">
         <f t="shared" si="13"/>
-        <v>-0.45095828633640167</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B43" s="3">
         <f t="shared" si="5"/>
-        <v>-0.45095828637789737</v>
+        <v>-0.22547914317920004</v>
       </c>
       <c r="C43" s="3">
         <f t="shared" si="6"/>
-        <v>-1.9397816686250735E-11</v>
+        <v>0.22547914317929951</v>
       </c>
       <c r="D43" s="3">
         <f t="shared" si="7"/>
-        <v>7.3280721532999991</v>
+        <v>7.5535512964986964</v>
       </c>
       <c r="E43" s="3">
         <f t="shared" si="8"/>
-        <v>1.3528748590561008</v>
+        <v>1.5783540022547982</v>
       </c>
       <c r="F43" s="3">
         <f t="shared" si="9"/>
-        <v>5.6369785794999956</v>
+        <v>5.8624577226986929</v>
       </c>
       <c r="G43" s="3">
         <f t="shared" si="10"/>
-        <v>1.2401352874999958</v>
+        <v>1.4656144306986931</v>
       </c>
       <c r="H43" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-0.56369785790130322</v>
       </c>
       <c r="I43" s="3">
         <f t="shared" si="12"/>
-        <v>0.77825852910000037</v>
+        <v>1.0037376722986977</v>
       </c>
       <c r="J43" s="3">
         <f t="shared" si="13"/>
-        <v>-0.22547914319869733</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B44" s="3">
         <f t="shared" si="5"/>
-        <v>2.2547914318080018</v>
+        <v>0.67643742953779906</v>
       </c>
       <c r="C44" s="3">
         <f t="shared" si="6"/>
-        <v>2.4802705749873013</v>
+        <v>0.90191657271709857</v>
       </c>
       <c r="D44" s="3">
         <f t="shared" si="7"/>
-        <v>9.2446448703999948</v>
+        <v>7.6662908681297921</v>
       </c>
       <c r="E44" s="3">
         <f t="shared" si="8"/>
-        <v>0.56369785796360361</v>
+        <v>-1.0146561443065991</v>
       </c>
       <c r="F44" s="3">
         <f t="shared" si="9"/>
-        <v>4.5095828636000022</v>
+        <v>2.9312288613297994</v>
       </c>
       <c r="G44" s="3">
         <f t="shared" si="10"/>
-        <v>2.4802705749999916</v>
+        <v>0.90191657272978887</v>
       </c>
       <c r="H44" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-1.352874859070198</v>
       </c>
       <c r="I44" s="3">
         <f t="shared" si="12"/>
-        <v>1.3429720589000027</v>
+        <v>-0.23538194337020002</v>
       </c>
       <c r="J44" s="3">
         <f t="shared" si="13"/>
-        <v>1.5783540022702027</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B45" s="3">
         <f t="shared" si="5"/>
-        <v>-0.22547914320529117</v>
+        <v>-0.33821871476889953</v>
       </c>
       <c r="C45" s="3">
         <f t="shared" si="6"/>
-        <v>-0.22547914320529117</v>
+        <v>-0.33821871476889953</v>
       </c>
       <c r="D45" s="3">
         <f t="shared" si="7"/>
-        <v>7.5535512965000038</v>
+        <v>7.4408117249363954</v>
       </c>
       <c r="E45" s="3">
         <f t="shared" si="8"/>
-        <v>2.8184892897147051</v>
+        <v>2.7057497181510968</v>
       </c>
       <c r="F45" s="3">
         <f t="shared" si="9"/>
-        <v>5.073280721499998</v>
+        <v>4.9605411499363896</v>
       </c>
       <c r="G45" s="3">
         <f t="shared" si="10"/>
-        <v>1.1273957158999934</v>
+        <v>1.0146561443363851</v>
       </c>
       <c r="H45" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.45095828633640167</v>
       </c>
       <c r="I45" s="3">
         <f t="shared" si="12"/>
-        <v>-1.5854637049999951</v>
+        <v>-1.6982032765636035</v>
       </c>
       <c r="J45" s="3">
         <f t="shared" si="13"/>
-        <v>0.11273957156360837</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B46" s="3">
         <f t="shared" si="5"/>
-        <v>2.5930101465806104</v>
+        <v>0.22547914317929951</v>
       </c>
       <c r="C46" s="3">
         <f t="shared" si="6"/>
-        <v>2.7057497181702104</v>
+        <v>0.33821871476889953</v>
       </c>
       <c r="D46" s="3">
         <f t="shared" si="7"/>
-        <v>9.244644870400009</v>
+        <v>6.8771138669986982</v>
       </c>
       <c r="E46" s="3">
         <f t="shared" si="8"/>
-        <v>4.0586245772458085</v>
+        <v>1.6910935738444977</v>
       </c>
       <c r="F46" s="3">
         <f t="shared" si="9"/>
-        <v>6.087936865900005</v>
+        <v>3.7204058624986942</v>
       </c>
       <c r="G46" s="3">
         <f t="shared" si="10"/>
-        <v>3.7204058625000158</v>
+        <v>1.352874859098705</v>
       </c>
       <c r="H46" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-0.22547914320129792</v>
       </c>
       <c r="I46" s="3">
         <f t="shared" si="12"/>
-        <v>4.2721695766000067</v>
+        <v>1.9046385731986959</v>
       </c>
       <c r="J46" s="3">
         <f t="shared" si="13"/>
-        <v>2.3675310034013108</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B47" s="3">
         <f t="shared" si="5"/>
-        <v>0.78917700112870648</v>
+        <v>0.11273957158960002</v>
       </c>
       <c r="C47" s="3">
         <f t="shared" si="6"/>
-        <v>0.56369785794950644</v>
+        <v>-0.11273957158960002</v>
       </c>
       <c r="D47" s="3">
         <f t="shared" si="7"/>
-        <v>7.1025930101000085</v>
+        <v>6.4261555805609021</v>
       </c>
       <c r="E47" s="3">
         <f t="shared" si="8"/>
-        <v>0.45095828635990642</v>
+        <v>-0.22547914317920004</v>
       </c>
       <c r="F47" s="3">
         <f t="shared" si="9"/>
-        <v>3.156708004500004</v>
+        <v>2.4802705749608975</v>
       </c>
       <c r="G47" s="3">
         <f t="shared" si="10"/>
-        <v>1.0146561442999911</v>
+        <v>0.33821871476088461</v>
       </c>
       <c r="H47" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-2.4802705749390981</v>
       </c>
       <c r="I47" s="3">
         <f t="shared" si="12"/>
-        <v>0.32806199659999891</v>
+        <v>-0.34837543293910755</v>
       </c>
       <c r="J47" s="3">
         <f t="shared" si="13"/>
-        <v>0.67643742953910646</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B48" s="3">
         <f t="shared" si="5"/>
-        <v>2.0293122886599093</v>
+        <v>-0.11273957158960002</v>
       </c>
       <c r="C48" s="3">
         <f t="shared" si="6"/>
-        <v>2.3675310034287094</v>
+        <v>0.22547914317920004</v>
       </c>
       <c r="D48" s="3">
         <f t="shared" si="7"/>
-        <v>7.4408117250000032</v>
+        <v>5.2987598647504939</v>
       </c>
       <c r="E48" s="3">
         <f t="shared" si="8"/>
-        <v>2.8184892897873084</v>
+        <v>0.67643742953779906</v>
       </c>
       <c r="F48" s="3">
         <f t="shared" si="9"/>
-        <v>6.6516347238000151</v>
+        <v>4.5095828635505057</v>
       </c>
       <c r="G48" s="3">
         <f t="shared" si="10"/>
-        <v>3.0439684330000034</v>
+        <v>0.90191657275049408</v>
       </c>
       <c r="H48" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-1.4656144306495094</v>
       </c>
       <c r="I48" s="3">
         <f t="shared" si="12"/>
-        <v>3.2577673503</v>
+        <v>1.1157154900504906</v>
       </c>
       <c r="J48" s="3">
         <f t="shared" si="13"/>
-        <v>2.1420518602495093</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B49" s="3">
         <f t="shared" si="5"/>
-        <v>-1.4656144307053012</v>
+        <v>-0.22547914317929951</v>
       </c>
       <c r="C49" s="3">
         <f t="shared" si="6"/>
-        <v>-1.3528748591157012</v>
+        <v>-0.11273957158969949</v>
       </c>
       <c r="D49" s="3">
         <f t="shared" si="7"/>
-        <v>7.2153325816999967</v>
+        <v>8.4554678692259984</v>
       </c>
       <c r="E49" s="3">
         <f t="shared" si="8"/>
-        <v>0.225479143139097</v>
+        <v>1.4656144306650987</v>
       </c>
       <c r="F49" s="3">
         <f t="shared" si="9"/>
-        <v>4.9605411498999956</v>
+        <v>6.2006764374259973</v>
       </c>
       <c r="G49" s="3">
         <f t="shared" si="10"/>
-        <v>0.90191657270000292</v>
+        <v>2.1420518602260046</v>
       </c>
       <c r="H49" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.67643742952598984</v>
       </c>
       <c r="I49" s="3">
         <f t="shared" si="12"/>
-        <v>1.0032298362999938</v>
+        <v>2.2433651238259955</v>
       </c>
       <c r="J49" s="3">
         <f t="shared" si="13"/>
-        <v>-1.2401352875260017</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B50" s="3">
         <f t="shared" si="5"/>
-        <v>-1.1273957159052941</v>
+        <v>0.22547914317929951</v>
       </c>
       <c r="C50" s="3">
         <f t="shared" si="6"/>
-        <v>-1.2401352874948941</v>
+        <v>0.11273957158969949</v>
       </c>
       <c r="D50" s="3">
         <f t="shared" si="7"/>
-        <v>6.4261555805999961</v>
+        <v>7.7790304396845897</v>
       </c>
       <c r="E50" s="3">
         <f t="shared" si="8"/>
-        <v>1.2401352874769032</v>
+        <v>2.5930101465614968</v>
       </c>
       <c r="F50" s="3">
         <f t="shared" si="9"/>
-        <v>5.9751972942000009</v>
+        <v>7.3280721532845945</v>
       </c>
       <c r="G50" s="3">
         <f t="shared" si="10"/>
-        <v>1.3528748590999982</v>
+        <v>2.7057497181845918</v>
       </c>
       <c r="H50" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.67643742958459541</v>
       </c>
       <c r="I50" s="3">
         <f t="shared" si="12"/>
-        <v>-0.46035325069999544</v>
+        <v>0.89252160838459815</v>
       </c>
       <c r="J50" s="3">
         <f t="shared" si="13"/>
-        <v>-1.3528748590845936</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B51" s="3">
         <f t="shared" si="5"/>
-        <v>0.4509582863325079</v>
+        <v>0.33821871476889953</v>
       </c>
       <c r="C51" s="3">
         <f t="shared" si="6"/>
-        <v>0.4509582863325079</v>
+        <v>0.33821871476889953</v>
       </c>
       <c r="D51" s="3">
         <f t="shared" si="7"/>
-        <v>6.6516347238000009</v>
+        <v>6.5388951522363925</v>
       </c>
       <c r="E51" s="3">
         <f t="shared" si="8"/>
-        <v>0.78917700110130795</v>
+        <v>0.67643742953769959</v>
       </c>
       <c r="F51" s="3">
         <f t="shared" si="9"/>
-        <v>4.5095828636000022</v>
+        <v>4.3968432920363938</v>
       </c>
       <c r="G51" s="3">
         <f t="shared" si="10"/>
-        <v>1.4656144305999987</v>
+        <v>1.3528748590363904</v>
       </c>
       <c r="H51" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.240135287436388</v>
       </c>
       <c r="I51" s="3">
         <f t="shared" si="12"/>
-        <v>-1.5854637049999951</v>
+        <v>-1.6982032765636035</v>
       </c>
       <c r="J51" s="3">
         <f t="shared" si="13"/>
-        <v>0.11273957156360837</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B52" s="3">
         <f t="shared" si="5"/>
-        <v>0.78917700111540512</v>
+        <v>-0.22547914317929951</v>
       </c>
       <c r="C52" s="3">
         <f t="shared" si="6"/>
-        <v>1.0146561442947046</v>
+        <v>0</v>
       </c>
       <c r="D52" s="3">
         <f t="shared" si="7"/>
-        <v>8.7936865839999996</v>
+        <v>7.779030439705295</v>
       </c>
       <c r="E52" s="3">
         <f t="shared" si="8"/>
-        <v>2.3675310033702033</v>
+        <v>1.3528748590754986</v>
       </c>
       <c r="F52" s="3">
         <f t="shared" si="9"/>
-        <v>4.2841037203999974</v>
+        <v>3.2694475761052928</v>
       </c>
       <c r="G52" s="3">
         <f t="shared" si="10"/>
-        <v>2.1420518601999987</v>
+        <v>1.1273957159052941</v>
       </c>
       <c r="H52" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.5783540022052875</v>
       </c>
       <c r="I52" s="3">
         <f t="shared" si="12"/>
-        <v>2.5825995104000015</v>
+        <v>1.5679433661052968</v>
       </c>
       <c r="J52" s="3">
         <f t="shared" si="13"/>
-        <v>1.0146561442947046</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B53" s="3">
         <f t="shared" si="5"/>
-        <v>-0.67643742957419306</v>
+        <v>0.33821871476889953</v>
       </c>
       <c r="C53" s="3">
         <f t="shared" si="6"/>
-        <v>-0.45095828639489355</v>
+        <v>0.56369785794819904</v>
       </c>
       <c r="D53" s="3">
         <f t="shared" si="7"/>
-        <v>5.1860202931000003</v>
+        <v>6.2006764374430929</v>
       </c>
       <c r="E53" s="3">
         <f t="shared" si="8"/>
-        <v>-0.45095828639489355</v>
+        <v>0.56369785794819904</v>
       </c>
       <c r="F53" s="3">
         <f t="shared" si="9"/>
-        <v>4.9605411498999956</v>
+        <v>5.9751972942430882</v>
       </c>
       <c r="G53" s="3">
         <f t="shared" si="10"/>
-        <v>0.90191657270000292</v>
+        <v>1.9165727170430955</v>
       </c>
       <c r="H53" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.4656144306431003</v>
       </c>
       <c r="I53" s="3">
         <f t="shared" si="12"/>
-        <v>0.7792742009000051</v>
+        <v>1.7939303452430977</v>
       </c>
       <c r="J53" s="3">
         <f t="shared" si="13"/>
-        <v>-1.0146561443430926</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B54" s="3">
         <f t="shared" si="5"/>
-        <v>-3.4949267192845923</v>
+        <v>-0.45095828635859903</v>
       </c>
       <c r="C54" s="3">
         <f t="shared" si="6"/>
-        <v>-3.7204058624637923</v>
+        <v>-0.67643742953779906</v>
       </c>
       <c r="D54" s="3">
         <f t="shared" si="7"/>
-        <v>5.1860202931000003</v>
+        <v>8.2299887260259936</v>
       </c>
       <c r="E54" s="3">
         <f t="shared" si="8"/>
-        <v>-1.3528748590815951</v>
+        <v>1.6910935738443982</v>
       </c>
       <c r="F54" s="3">
         <f t="shared" si="9"/>
-        <v>1.6910935738000035</v>
+        <v>4.7350620067259968</v>
       </c>
       <c r="G54" s="3">
         <f t="shared" si="10"/>
-        <v>1.0146561443000053</v>
+        <v>4.0586245772259986</v>
       </c>
       <c r="H54" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.22547914322599638</v>
       </c>
       <c r="I54" s="3">
         <f t="shared" si="12"/>
-        <v>-1.4762789847000022</v>
+        <v>1.5676894482259911</v>
       </c>
       <c r="J54" s="3">
         <f t="shared" si="13"/>
-        <v>-3.0439684329259933</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B55" s="3">
         <f t="shared" si="5"/>
-        <v>-0.33821871474680165</v>
+        <v>0.67643742953779906</v>
       </c>
       <c r="C55" s="3">
         <f t="shared" si="6"/>
-        <v>0.22547914320129792</v>
+        <v>1.2401352874858986</v>
       </c>
       <c r="D55" s="3">
         <f t="shared" si="7"/>
-        <v>5.0732807215999998</v>
+        <v>6.0879368658846005</v>
       </c>
       <c r="E55" s="3">
         <f t="shared" si="8"/>
-        <v>1.9165727170457956</v>
+        <v>2.9312288613303963</v>
       </c>
       <c r="F55" s="3">
         <f t="shared" si="9"/>
-        <v>5.4114994362999909</v>
+        <v>6.4261555805845916</v>
       </c>
       <c r="G55" s="3">
         <f t="shared" si="10"/>
-        <v>1.916572716999994</v>
+        <v>2.9312288612845947</v>
       </c>
       <c r="H55" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-0.33821871481541166</v>
       </c>
       <c r="I55" s="3">
         <f t="shared" si="12"/>
-        <v>-0.57258498630000076</v>
+        <v>0.44207115798459995</v>
       </c>
       <c r="J55" s="3">
         <f t="shared" si="13"/>
-        <v>-1.0146561442846007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B56" s="3">
         <f t="shared" si="5"/>
-        <v>0.78917700116360834</v>
+        <v>0.45095828635849955</v>
       </c>
       <c r="C56" s="3">
         <f t="shared" si="6"/>
-        <v>0.56369785798430883</v>
+        <v>0.22547914317920004</v>
       </c>
       <c r="D56" s="3">
         <f t="shared" si="7"/>
-        <v>8.3427282977000061</v>
+        <v>8.0045095828948973</v>
       </c>
       <c r="E56" s="3">
         <f t="shared" si="8"/>
-        <v>1.9165727170599069</v>
+        <v>1.5783540022547982</v>
       </c>
       <c r="F56" s="3">
         <f t="shared" si="9"/>
-        <v>5.749718151099998</v>
+        <v>5.4114994362948892</v>
       </c>
       <c r="G56" s="3">
         <f t="shared" si="10"/>
-        <v>3.7204058625000016</v>
+        <v>3.3821871476948928</v>
       </c>
       <c r="H56" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.22547914319488882</v>
       </c>
       <c r="I56" s="3">
         <f t="shared" si="12"/>
-        <v>4.04592867960001</v>
+        <v>3.7077099647949012</v>
       </c>
       <c r="J56" s="3">
         <f t="shared" si="13"/>
-        <v>0.33821871480510879</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B57" s="3">
         <f t="shared" si="5"/>
-        <v>0.90191657274280601</v>
+        <v>0.9019165727169991</v>
       </c>
       <c r="C57" s="3">
         <f t="shared" si="6"/>
-        <v>1.2401352875117055</v>
+        <v>1.2401352874858986</v>
       </c>
       <c r="D57" s="3">
         <f t="shared" si="7"/>
-        <v>6.4261555805999961</v>
+        <v>6.4261555805741892</v>
       </c>
       <c r="E57" s="3">
         <f t="shared" si="8"/>
-        <v>2.2547914318184041</v>
+        <v>2.2547914317925972</v>
       </c>
       <c r="F57" s="3">
         <f t="shared" si="9"/>
-        <v>6.087936865900005</v>
+        <v>6.0879368658741981</v>
       </c>
       <c r="G57" s="3">
         <f t="shared" si="10"/>
-        <v>3.2694475760999921</v>
+        <v>3.2694475760741852</v>
       </c>
       <c r="H57" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.2401352874741889</v>
       </c>
       <c r="I57" s="3">
         <f t="shared" si="12"/>
-        <v>3.0322882070999952</v>
+        <v>3.0322882070741883</v>
       </c>
       <c r="J57" s="3">
         <f t="shared" si="13"/>
-        <v>2.5806912162806839E-11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B58" s="3">
         <f t="shared" si="5"/>
-        <v>0.67643742949471175</v>
+        <v>0.56369785794809957</v>
       </c>
       <c r="C58" s="3">
         <f t="shared" si="6"/>
-        <v>0.56369785790511173</v>
+        <v>0.45095828635849955</v>
       </c>
       <c r="D58" s="3">
         <f t="shared" si="7"/>
-        <v>8.229988726000002</v>
+        <v>8.1172491544533898</v>
       </c>
       <c r="E58" s="3">
         <f t="shared" si="8"/>
-        <v>2.3675310033391099</v>
+        <v>2.2547914317924977</v>
       </c>
       <c r="F58" s="3">
         <f t="shared" si="9"/>
-        <v>7.3280721533000133</v>
+        <v>7.2153325817534011</v>
       </c>
       <c r="G58" s="3">
         <f t="shared" si="10"/>
-        <v>3.720405862400014</v>
+        <v>3.6076662908534018</v>
       </c>
       <c r="H58" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.2401352874533984</v>
       </c>
       <c r="I58" s="3">
         <f t="shared" si="12"/>
-        <v>2.6948312461000086</v>
+        <v>2.5820916745533964</v>
       </c>
       <c r="J58" s="3">
         <f t="shared" si="13"/>
-        <v>0.11273957154661218</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B59" s="3">
         <f t="shared" si="5"/>
-        <v>0.78917700110130795</v>
+        <v>0.22547914317920004</v>
       </c>
       <c r="C59" s="3">
         <f t="shared" si="6"/>
-        <v>0.78917700110130795</v>
+        <v>0.22547914317920004</v>
       </c>
       <c r="D59" s="3">
         <f t="shared" si="7"/>
-        <v>7.6662908681000062</v>
+        <v>7.1025930101778982</v>
       </c>
       <c r="E59" s="3">
         <f t="shared" si="8"/>
-        <v>2.3675310033561061</v>
+        <v>1.8038331454339982</v>
       </c>
       <c r="F59" s="3">
         <f t="shared" si="9"/>
-        <v>6.4261555806000104</v>
+        <v>5.8624577226779024</v>
       </c>
       <c r="G59" s="3">
         <f t="shared" si="10"/>
-        <v>2.8184892897000111</v>
+        <v>2.2547914317779032</v>
       </c>
       <c r="H59" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-1.2401352875221079</v>
       </c>
       <c r="I59" s="3">
         <f t="shared" si="12"/>
-        <v>3.36949125000001</v>
+        <v>2.8057933920779021</v>
       </c>
       <c r="J59" s="3">
         <f t="shared" si="13"/>
-        <v>0.56369785792210791</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B60" s="3">
         <f t="shared" si="5"/>
-        <v>1.9165727169806104</v>
+        <v>0.11273957158960002</v>
       </c>
       <c r="C60" s="3">
         <f t="shared" si="6"/>
-        <v>2.3675310033391099</v>
+        <v>0.56369785794809957</v>
       </c>
       <c r="D60" s="3">
         <f t="shared" si="7"/>
-        <v>7.7790304396000067</v>
+        <v>5.9751972942089964</v>
       </c>
       <c r="E60" s="3">
         <f t="shared" si="8"/>
-        <v>1.2401352874428113</v>
+        <v>-0.56369785794819904</v>
       </c>
       <c r="F60" s="3">
         <f t="shared" si="9"/>
-        <v>9.3573844419000096</v>
+        <v>7.5535512965089993</v>
       </c>
       <c r="G60" s="3">
         <f t="shared" si="10"/>
-        <v>3.9458850056000045</v>
+        <v>2.1420518602089942</v>
       </c>
       <c r="H60" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.33821871480900256</v>
       </c>
       <c r="I60" s="3">
         <f t="shared" si="12"/>
-        <v>1.3434798947000104</v>
+        <v>-0.46035325069099997</v>
       </c>
       <c r="J60" s="3">
         <f t="shared" si="13"/>
-        <v>1.8038331453910104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B61" s="3">
         <f t="shared" si="5"/>
-        <v>2.0293122886183994</v>
+        <v>0.45095828635849955</v>
       </c>
       <c r="C61" s="3">
         <f t="shared" si="6"/>
-        <v>2.2547914317975994</v>
+        <v>0.67643742953769959</v>
       </c>
       <c r="D61" s="3">
         <f t="shared" si="7"/>
-        <v>6.8771138669999914</v>
+        <v>5.2987598647400915</v>
       </c>
       <c r="E61" s="3">
         <f t="shared" si="8"/>
-        <v>1.1273957159013008</v>
+        <v>-0.45095828635859903</v>
       </c>
       <c r="F61" s="3">
         <f t="shared" si="9"/>
-        <v>6.5388951521999985</v>
+        <v>4.9605411499400986</v>
       </c>
       <c r="G61" s="3">
         <f t="shared" si="10"/>
-        <v>2.7057497181999963</v>
+        <v>1.1273957159400965</v>
       </c>
       <c r="H61" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-1.1273957158599046</v>
       </c>
       <c r="I61" s="3">
         <f t="shared" si="12"/>
-        <v>3.2572595143000029</v>
+        <v>1.6789055120401031</v>
       </c>
       <c r="J61" s="3">
         <f t="shared" si="13"/>
-        <v>1.5783540022598999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B62" s="3">
         <f t="shared" si="5"/>
-        <v>2.3675310034184065</v>
+        <v>-0.22547914317920004</v>
       </c>
       <c r="C62" s="3">
         <f t="shared" si="6"/>
-        <v>3.0439684329561061</v>
+        <v>0.45095828635849955</v>
       </c>
       <c r="D62" s="3">
         <f t="shared" si="7"/>
-        <v>7.5535512965000038</v>
+        <v>4.9605411499023973</v>
       </c>
       <c r="E62" s="3">
         <f t="shared" si="8"/>
-        <v>1.1273957159325079</v>
+        <v>-1.4656144306650987</v>
       </c>
       <c r="F62" s="3">
         <f t="shared" si="9"/>
-        <v>6.5388951522000127</v>
+        <v>3.9458850056024062</v>
       </c>
       <c r="G62" s="3">
         <f t="shared" si="10"/>
-        <v>1.6910935739000053</v>
+        <v>-0.90191657269760128</v>
       </c>
       <c r="H62" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-1.6910935737976018</v>
       </c>
       <c r="I62" s="3">
         <f t="shared" si="12"/>
-        <v>3.3702530039000038</v>
+        <v>0.77724285730239728</v>
       </c>
       <c r="J62" s="3">
         <f t="shared" si="13"/>
-        <v>2.5930101465976065</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B63" s="3">
         <f t="shared" si="5"/>
-        <v>-0.56369785793638982</v>
+        <v>0.33821871476889953</v>
       </c>
       <c r="C63" s="3">
         <f t="shared" si="6"/>
-        <v>-0.11273957157789027</v>
+        <v>0.78917700112739908</v>
       </c>
       <c r="D63" s="3">
         <f t="shared" si="7"/>
-        <v>6.313416009000008</v>
+        <v>7.2153325817052973</v>
       </c>
       <c r="E63" s="3">
         <f t="shared" si="8"/>
-        <v>-0.22547914316749029</v>
+        <v>0.67643742953779906</v>
       </c>
       <c r="F63" s="3">
         <f t="shared" si="9"/>
-        <v>4.8478015784000092</v>
+        <v>5.7497181511052986</v>
       </c>
       <c r="G63" s="3">
         <f t="shared" si="10"/>
-        <v>1.6910935739000053</v>
+        <v>2.5930101466052946</v>
       </c>
       <c r="H63" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.6910935738052899</v>
       </c>
       <c r="I63" s="3">
         <f t="shared" si="12"/>
-        <v>1.5669276943000057</v>
+        <v>2.468844267005295</v>
       </c>
       <c r="J63" s="3">
         <f t="shared" si="13"/>
-        <v>-0.90191657270528935</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B64" s="3">
         <f t="shared" si="5"/>
-        <v>0.22547914321540929</v>
+        <v>0</v>
       </c>
       <c r="C64" s="3">
         <f t="shared" si="6"/>
-        <v>0.45095828639470881</v>
+        <v>0.22547914317929951</v>
       </c>
       <c r="D64" s="3">
         <f t="shared" si="7"/>
-        <v>8.9064261556000019</v>
+        <v>8.6809470123845927</v>
       </c>
       <c r="E64" s="3">
         <f t="shared" si="8"/>
-        <v>1.5783540022910074</v>
+        <v>1.3528748590755981</v>
       </c>
       <c r="F64" s="3">
         <f t="shared" si="9"/>
-        <v>7.2153325817999985</v>
+        <v>6.9898534385845892</v>
       </c>
       <c r="G64" s="3">
         <f t="shared" si="10"/>
-        <v>1.6910935739000053</v>
+        <v>1.465614430684596</v>
       </c>
       <c r="H64" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.56369785798459304</v>
       </c>
       <c r="I64" s="3">
         <f t="shared" si="12"/>
-        <v>2.2441268777999994</v>
+        <v>2.0186477345845901</v>
       </c>
       <c r="J64" s="3">
         <f t="shared" si="13"/>
-        <v>0.22547914321540929</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B65" s="3">
         <f t="shared" si="5"/>
-        <v>0.56369785799471117</v>
+        <v>0.56369785794809957</v>
       </c>
       <c r="C65" s="3">
         <f t="shared" si="6"/>
-        <v>0.11273957163621162</v>
+        <v>0.11273957158960002</v>
       </c>
       <c r="D65" s="3">
         <f t="shared" si="7"/>
-        <v>7.2153325818000127</v>
+        <v>7.2153325817534011</v>
       </c>
       <c r="E65" s="3">
         <f t="shared" si="8"/>
-        <v>1.2401352875325102</v>
+        <v>1.2401352874858986</v>
       </c>
       <c r="F65" s="3">
         <f t="shared" si="9"/>
-        <v>6.2006764375000074</v>
+        <v>6.2006764374533958</v>
       </c>
       <c r="G65" s="3">
         <f t="shared" si="10"/>
-        <v>3.2694475761000064</v>
+        <v>3.2694475760533948</v>
       </c>
       <c r="H65" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.9019165727533931</v>
       </c>
       <c r="I65" s="3">
         <f t="shared" si="12"/>
-        <v>3.9334430259000044</v>
+        <v>3.9334430258533928</v>
       </c>
       <c r="J65" s="3">
         <f t="shared" si="13"/>
-        <v>4.6611603465862572E-11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B66" s="3">
         <f t="shared" si="5"/>
-        <v>1.2401352874531995</v>
+        <v>0.56369785794809957</v>
       </c>
       <c r="C66" s="3">
         <f t="shared" si="6"/>
-        <v>1.2401352874531995</v>
+        <v>0.56369785794809957</v>
       </c>
       <c r="D66" s="3">
         <f t="shared" si="7"/>
-        <v>10.935738444199998</v>
+        <v>10.259301014694898</v>
       </c>
       <c r="E66" s="3">
         <f t="shared" si="8"/>
-        <v>2.9312288612975976</v>
+        <v>2.2547914317924977</v>
       </c>
       <c r="F66" s="3">
         <f t="shared" si="9"/>
-        <v>6.8771138669000038</v>
+        <v>6.2006764373949039</v>
       </c>
       <c r="G66" s="3">
         <f t="shared" si="10"/>
-        <v>2.9312288612999993</v>
+        <v>2.2547914317948994</v>
       </c>
       <c r="H66" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-0.11273957160510406</v>
       </c>
       <c r="I66" s="3">
         <f t="shared" si="12"/>
-        <v>2.1318951419999905</v>
+        <v>1.4554577124948906</v>
       </c>
       <c r="J66" s="3">
         <f t="shared" si="13"/>
-        <v>0.67643742950509989</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>